<commit_message>
feat: Add shipment document management and invoicing features
- Introduced a new model `shipment.document` to track required documents for shipments.
- Added views for managing shipment documents including kanban, list, and form views.
- Enhanced `shipment_request` model with fields for proforma and invoice management.
- Implemented methods for creating proforma invoices and handling transport fees.
- Updated the manifest to include new data files and views.
- Added security access rights for shipment documents.
- Enhanced the shipment request form to include document and invoicing information.
- Created XML data for transport service products.
</commit_message>
<xml_diff>
--- a/custom_fleet_fuel_management/docs/template_import_depenses_carburant.xlsx
+++ b/custom_fleet_fuel_management/docs/template_import_depenses_carburant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Import Depenses"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>GUIDE IMPORT DEPENSES CARBURANT</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>2. Doublons detectes automatiquement</t>
-  </si>
-  <si>
-    <t>3. Supprimer ligne 2 avant import</t>
   </si>
   <si>
     <t>card_uid</t>
@@ -122,7 +119,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -134,7 +131,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -221,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,6 +252,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -566,48 +566,48 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="30.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="10">
         <v>75.5</v>
@@ -616,21 +616,21 @@
         <v>50.25</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="11">
         <v>125430</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C3" s="11">
         <v>45</v>
@@ -639,19 +639,19 @@
         <v>30.15</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="11">
         <v>125890</v>
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="10">
         <v>82.3</v>
@@ -660,13 +660,13 @@
         <v>55</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="11">
         <v>89120</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -679,9 +679,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -762,11 +762,6 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>